<commit_message>
actualise test xlsx and main.py
</commit_message>
<xml_diff>
--- a/dataTest/fichier_excel.xlsx
+++ b/dataTest/fichier_excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="146">
   <si>
     <t>n_position</t>
   </si>
@@ -94,9 +94,6 @@
     <t>00861</t>
   </si>
   <si>
-    <t>Contrôle1</t>
-  </si>
-  <si>
     <t>Contrôle</t>
   </si>
   <si>
@@ -250,12 +247,6 @@
     <t>00890</t>
   </si>
   <si>
-    <t>Contrôle2</t>
-  </si>
-  <si>
-    <t>Contrôle3</t>
-  </si>
-  <si>
     <t>0780</t>
   </si>
   <si>
@@ -368,9 +359,6 @@
   </si>
   <si>
     <t>00916</t>
-  </si>
-  <si>
-    <t>Contrôle4</t>
   </si>
   <si>
     <t>0799</t>
@@ -888,7 +876,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="17.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="11" width="9.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="12" width="8.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
@@ -1055,10 +1043,10 @@
         <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1066,10 +1054,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>11</v>
@@ -1080,10 +1068,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>6</v>
@@ -1094,10 +1082,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>6</v>
@@ -1108,10 +1096,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>6</v>
@@ -1122,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>6</v>
@@ -1136,10 +1124,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
@@ -1150,10 +1138,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>6</v>
@@ -1164,10 +1152,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>6</v>
@@ -1178,10 +1166,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>6</v>
@@ -1192,13 +1180,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -1206,10 +1194,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>6</v>
@@ -1220,10 +1208,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>6</v>
@@ -1234,10 +1222,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>6</v>
@@ -1248,10 +1236,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>6</v>
@@ -1262,10 +1250,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>6</v>
@@ -1276,10 +1264,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>6</v>
@@ -1290,10 +1278,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>6</v>
@@ -1304,10 +1292,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>6</v>
@@ -1318,10 +1306,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>6</v>
@@ -1332,10 +1320,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>6</v>
@@ -1346,10 +1334,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>6</v>
@@ -1360,10 +1348,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>6</v>
@@ -1374,10 +1362,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>6</v>
@@ -1388,10 +1376,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>6</v>
@@ -1402,13 +1390,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
@@ -1416,13 +1404,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
@@ -1430,10 +1418,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>6</v>
@@ -1444,10 +1432,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>6</v>
@@ -1458,10 +1446,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>6</v>
@@ -1472,10 +1460,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>6</v>
@@ -1486,10 +1474,10 @@
         <v>6</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>6</v>
@@ -1500,10 +1488,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>6</v>
@@ -1514,10 +1502,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>6</v>
@@ -1528,10 +1516,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>6</v>
@@ -1542,10 +1530,10 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>6</v>
@@ -1556,10 +1544,10 @@
         <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>6</v>
@@ -1570,10 +1558,10 @@
         <v>12</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>6</v>
@@ -1584,10 +1572,10 @@
         <v>13</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>6</v>
@@ -1598,10 +1586,10 @@
         <v>14</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>6</v>
@@ -1612,10 +1600,10 @@
         <v>15</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>6</v>
@@ -1626,10 +1614,10 @@
         <v>16</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>11</v>
@@ -1640,10 +1628,10 @@
         <v>17</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>6</v>
@@ -1654,10 +1642,10 @@
         <v>18</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>6</v>
@@ -1668,10 +1656,10 @@
         <v>19</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>6</v>
@@ -1682,10 +1670,10 @@
         <v>20</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>6</v>
@@ -1696,13 +1684,13 @@
         <v>21</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>118</v>
+        <v>26</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -1710,10 +1698,10 @@
         <v>22</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>6</v>
@@ -1724,10 +1712,10 @@
         <v>23</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>6</v>
@@ -1738,10 +1726,10 @@
         <v>24</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>11</v>
@@ -1752,10 +1740,10 @@
         <v>25</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>6</v>
@@ -1766,13 +1754,13 @@
         <v>26</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -1780,10 +1768,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>6</v>
@@ -1794,10 +1782,10 @@
         <v>28</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>6</v>
@@ -1808,10 +1796,10 @@
         <v>29</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>6</v>
@@ -1822,10 +1810,10 @@
         <v>30</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>6</v>
@@ -1836,10 +1824,10 @@
         <v>31</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>6</v>
@@ -1850,10 +1838,10 @@
         <v>32</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>6</v>
@@ -1864,10 +1852,10 @@
         <v>33</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>6</v>
@@ -1878,10 +1866,10 @@
         <v>34</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>6</v>
@@ -1892,10 +1880,10 @@
         <v>35</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>6</v>
@@ -1906,10 +1894,10 @@
         <v>36</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>6</v>

</xml_diff>